<commit_message>
Update with INTENT 2023
</commit_message>
<xml_diff>
--- a/INTIS/INTIS.xlsx
+++ b/INTIS/INTIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linfri/Projects/INTIS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linfri/LRF/INTENT-main/INTIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C0F8E0-9BEC-BB4A-AEEB-8FF65DD68C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C886BC31-3639-8345-A47F-705FEC27934D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{47619717-D1F4-094D-8B7F-F898BC48ECF7}"/>
+    <workbookView xWindow="600" yWindow="5760" windowWidth="28040" windowHeight="9920" xr2:uid="{47619717-D1F4-094D-8B7F-F898BC48ECF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="179">
   <si>
     <t>Year</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Ireland</t>
   </si>
   <si>
-    <t>Linn Friberg</t>
-  </si>
-  <si>
     <t>Chris DeBry</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>DJ_Iterate</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>DJ_Frankenstone</t>
   </si>
   <si>
@@ -392,6 +386,192 @@
   </si>
   <si>
     <t>Neal D. Retke</t>
+  </si>
+  <si>
+    <t>Akkamiau</t>
+  </si>
+  <si>
+    <t>Sarah Martinus</t>
+  </si>
+  <si>
+    <t>Dominik t'Jolle</t>
+  </si>
+  <si>
+    <t>Jena Jang</t>
+  </si>
+  <si>
+    <t>LR Friberg</t>
+  </si>
+  <si>
+    <t>Piet Schen</t>
+  </si>
+  <si>
+    <t>Autonomaton</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Coyote Senate</t>
+  </si>
+  <si>
+    <t>Voiwode</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Melophobia</t>
+  </si>
+  <si>
+    <t>Skyler Remillard</t>
+  </si>
+  <si>
+    <t>Ahrien</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Ohmnoise</t>
+  </si>
+  <si>
+    <t>chra</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Scott Roller</t>
+  </si>
+  <si>
+    <t>Filmy Ghost</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Jaime Munárriz</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Der Allgegenwärtige Astronautenstamm</t>
+  </si>
+  <si>
+    <t>Stefan Strasser</t>
+  </si>
+  <si>
+    <t>Catenation</t>
+  </si>
+  <si>
+    <t>Ben Coudert</t>
+  </si>
+  <si>
+    <t>Antonella Eye Porcelluzzi</t>
+  </si>
+  <si>
+    <t>Steffi Baron-Neuhuber</t>
+  </si>
+  <si>
+    <t>Elektronengehirn</t>
+  </si>
+  <si>
+    <t>Wayne DeFehr</t>
+  </si>
+  <si>
+    <t>Obhod</t>
+  </si>
+  <si>
+    <t>Genda</t>
+  </si>
+  <si>
+    <t>Roboknob</t>
+  </si>
+  <si>
+    <t>V-Stók</t>
+  </si>
+  <si>
+    <t>Jon Shuemaker</t>
+  </si>
+  <si>
+    <t>Signals From Sirius</t>
+  </si>
+  <si>
+    <t>D-Fried</t>
+  </si>
+  <si>
+    <t>Mediatrix</t>
+  </si>
+  <si>
+    <t>Notstandskomitee</t>
+  </si>
+  <si>
+    <t>Forest Lake</t>
+  </si>
+  <si>
+    <t>Ana María Romano G.</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Story Of The Lie</t>
+  </si>
+  <si>
+    <t>Helecho Experimentar</t>
+  </si>
+  <si>
+    <t>PDMF</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>SonoroNoise</t>
+  </si>
+  <si>
+    <t>Humanfobia</t>
+  </si>
+  <si>
+    <t>Toshiro Koreshina</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>IMPROCITY</t>
+  </si>
+  <si>
+    <t>Axis Project</t>
+  </si>
+  <si>
+    <t>Hironaka Tokuma</t>
+  </si>
+  <si>
+    <t>Crystal Creek</t>
+  </si>
+  <si>
+    <t>Resitant</t>
+  </si>
+  <si>
+    <t>El Zombie Espacial</t>
+  </si>
+  <si>
+    <t>Nina Kardec</t>
+  </si>
+  <si>
+    <t>flyoversx</t>
+  </si>
+  <si>
+    <t>Tom Chapman</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Greenland</t>
   </si>
 </sst>
 </file>
@@ -751,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796CDF84-337F-F644-868D-9505BC8FAD2B}">
-  <dimension ref="A1:P147"/>
+  <dimension ref="A1:P267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="D244" sqref="D244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,22 +944,22 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>102</v>
-      </c>
-      <c r="E1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -788,28 +968,28 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>109</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>110</v>
-      </c>
-      <c r="O1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -831,7 +1011,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G3">
         <v>2020</v>
@@ -845,7 +1025,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G4">
         <v>2020</v>
@@ -887,7 +1067,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G7">
         <v>2020</v>
@@ -929,7 +1109,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G10">
         <v>2020</v>
@@ -949,7 +1129,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -992,7 +1172,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -1077,7 +1257,7 @@
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G18">
         <v>2020</v>
@@ -1111,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G20">
         <v>2020</v>
@@ -1229,13 +1409,13 @@
         <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G28">
         <v>2020</v>
@@ -1263,7 +1443,7 @@
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G30">
         <v>2020</v>
@@ -1394,7 +1574,7 @@
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G38">
         <v>2021</v>
@@ -1519,7 +1699,7 @@
         <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G46">
         <v>2021</v>
@@ -1567,7 +1747,7 @@
         <v>53</v>
       </c>
       <c r="D49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G49">
         <v>2021</v>
@@ -1581,7 +1761,7 @@
         <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G50">
         <v>2021</v>
@@ -1671,7 +1851,7 @@
         <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G56">
         <v>2021</v>
@@ -1699,7 +1879,7 @@
         <v>59</v>
       </c>
       <c r="D58" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G58">
         <v>2021</v>
@@ -1724,16 +1904,16 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" t="s">
         <v>62</v>
-      </c>
-      <c r="B60" t="s">
-        <v>63</v>
       </c>
       <c r="D60" t="s">
         <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G60">
         <v>2021</v>
@@ -1744,10 +1924,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G61">
         <v>2021</v>
@@ -1775,7 +1955,7 @@
         <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -1792,10 +1972,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G64">
         <v>2021</v>
@@ -1834,7 +2014,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67" t="s">
         <v>9</v>
@@ -1848,10 +2028,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G68">
         <v>2021</v>
@@ -1865,7 +2045,7 @@
         <v>54</v>
       </c>
       <c r="D69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G69">
         <v>2021</v>
@@ -1876,10 +2056,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D70" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G70">
         <v>2021</v>
@@ -1890,10 +2070,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G71">
         <v>2021</v>
@@ -1932,10 +2112,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D74" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G74">
         <v>2021</v>
@@ -1946,7 +2126,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D75" t="s">
         <v>36</v>
@@ -1960,10 +2140,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D76" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G76">
         <v>2021</v>
@@ -1974,10 +2154,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D77" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G77">
         <v>2021</v>
@@ -2002,7 +2182,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D79" t="s">
         <v>36</v>
@@ -2016,10 +2196,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D80" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G80">
         <v>2021</v>
@@ -2030,10 +2210,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D81" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G81">
         <v>2021</v>
@@ -2047,7 +2227,7 @@
         <v>4</v>
       </c>
       <c r="D82" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G82">
         <v>2021</v>
@@ -2058,10 +2238,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D83" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G83">
         <v>2021</v>
@@ -2075,7 +2255,7 @@
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G84">
         <v>2021</v>
@@ -2086,10 +2266,10 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D85" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G85">
         <v>2021</v>
@@ -2100,10 +2280,10 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D86" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G86">
         <v>2021</v>
@@ -2114,7 +2294,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D87" t="s">
         <v>16</v>
@@ -2128,10 +2308,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D88" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G88">
         <v>2021</v>
@@ -2142,7 +2322,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>16</v>
@@ -2156,10 +2336,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D90" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G90">
         <v>2021</v>
@@ -2170,7 +2350,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D91" t="s">
         <v>16</v>
@@ -2201,7 +2381,7 @@
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G93">
         <v>2021</v>
@@ -2212,10 +2392,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D94" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G94">
         <v>2021</v>
@@ -2226,10 +2406,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D95" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G95">
         <v>2021</v>
@@ -2243,7 +2423,7 @@
         <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G96">
         <v>2021</v>
@@ -2285,7 +2465,7 @@
         <v>53</v>
       </c>
       <c r="D99" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G99">
         <v>2021</v>
@@ -2310,10 +2490,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D101" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G101">
         <v>2022</v>
@@ -2324,10 +2504,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D102" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G102">
         <v>2022</v>
@@ -2352,10 +2532,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D104" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G104">
         <v>2022</v>
@@ -2380,10 +2560,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D106" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G106">
         <v>2022</v>
@@ -2397,7 +2577,7 @@
         <v>51</v>
       </c>
       <c r="D107" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G107">
         <v>2022</v>
@@ -2408,10 +2588,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D108" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G108">
         <v>2022</v>
@@ -2422,7 +2602,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D109" t="s">
         <v>61</v>
@@ -2436,10 +2616,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D110" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G110">
         <v>2022</v>
@@ -2450,10 +2630,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D111" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G111">
         <v>2022</v>
@@ -2478,10 +2658,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D113" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G113">
         <v>2022</v>
@@ -2506,13 +2686,13 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B115" t="s">
         <v>14</v>
       </c>
       <c r="D115" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E115" t="s">
         <v>16</v>
@@ -2526,10 +2706,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D116" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G116">
         <v>2022</v>
@@ -2540,7 +2720,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D117" t="s">
         <v>42</v>
@@ -2554,10 +2734,10 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D118" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G118">
         <v>2022</v>
@@ -2571,7 +2751,7 @@
         <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G119">
         <v>2022</v>
@@ -2599,7 +2779,7 @@
         <v>5</v>
       </c>
       <c r="D121" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G121">
         <v>2022</v>
@@ -2613,7 +2793,7 @@
         <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G122">
         <v>2022</v>
@@ -2641,7 +2821,7 @@
         <v>54</v>
       </c>
       <c r="D124" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G124">
         <v>2022</v>
@@ -2655,7 +2835,7 @@
         <v>4</v>
       </c>
       <c r="D125" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G125">
         <v>2022</v>
@@ -2666,10 +2846,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D126" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G126">
         <v>2022</v>
@@ -2683,7 +2863,7 @@
         <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G127">
         <v>2022</v>
@@ -2725,7 +2905,7 @@
         <v>43</v>
       </c>
       <c r="D130" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G130">
         <v>2022</v>
@@ -2750,10 +2930,10 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D132" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G132">
         <v>2022</v>
@@ -2778,10 +2958,10 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G134">
         <v>2022</v>
@@ -2806,7 +2986,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D136" t="s">
         <v>61</v>
@@ -2820,13 +3000,13 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B137" t="s">
         <v>60</v>
       </c>
       <c r="C137" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D137" t="s">
         <v>61</v>
@@ -2835,7 +3015,7 @@
         <v>61</v>
       </c>
       <c r="F137" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G137">
         <v>2022</v>
@@ -2844,42 +3024,42 @@
         <v>5</v>
       </c>
       <c r="I137" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="J137" t="s">
         <v>16</v>
       </c>
       <c r="K137" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L137" t="s">
         <v>36</v>
       </c>
       <c r="M137" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N137" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O137" t="s">
         <v>59</v>
       </c>
       <c r="P137" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B138" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D138" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G138">
         <v>2022</v>
@@ -2890,7 +3070,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="D139" t="s">
         <v>16</v>
@@ -2907,7 +3087,7 @@
         <v>4</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G140">
         <v>2022</v>
@@ -2918,7 +3098,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D141" t="s">
         <v>36</v>
@@ -2932,7 +3112,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="D142" t="s">
         <v>16</v>
@@ -2960,7 +3140,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D144" t="s">
         <v>36</v>
@@ -2972,9 +3152,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D145" t="s">
         <v>36</v>
@@ -2986,12 +3166,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B146" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="D146" t="s">
         <v>36</v>
@@ -3006,24 +3186,1824 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B147" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D147" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G147">
         <v>2022</v>
       </c>
       <c r="H147">
         <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>117</v>
+      </c>
+      <c r="B148" t="s">
+        <v>60</v>
+      </c>
+      <c r="C148" t="s">
+        <v>119</v>
+      </c>
+      <c r="D148" t="s">
+        <v>9</v>
+      </c>
+      <c r="E148" t="s">
+        <v>61</v>
+      </c>
+      <c r="F148" t="s">
+        <v>36</v>
+      </c>
+      <c r="G148">
+        <v>2023</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+      <c r="I148" t="s">
+        <v>92</v>
+      </c>
+      <c r="J148" t="s">
+        <v>93</v>
+      </c>
+      <c r="K148" t="s">
+        <v>120</v>
+      </c>
+      <c r="L148" t="s">
+        <v>177</v>
+      </c>
+      <c r="M148" t="s">
+        <v>121</v>
+      </c>
+      <c r="N148" t="s">
+        <v>16</v>
+      </c>
+      <c r="O148" t="s">
+        <v>122</v>
+      </c>
+      <c r="P148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>121</v>
+      </c>
+      <c r="D149" t="s">
+        <v>16</v>
+      </c>
+      <c r="G149">
+        <v>2023</v>
+      </c>
+      <c r="H149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>123</v>
+      </c>
+      <c r="D150" t="s">
+        <v>124</v>
+      </c>
+      <c r="G150">
+        <v>2023</v>
+      </c>
+      <c r="H150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>125</v>
+      </c>
+      <c r="D151" t="s">
+        <v>111</v>
+      </c>
+      <c r="G151">
+        <v>2023</v>
+      </c>
+      <c r="H151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>126</v>
+      </c>
+      <c r="D152" t="s">
+        <v>127</v>
+      </c>
+      <c r="G152">
+        <v>2023</v>
+      </c>
+      <c r="H152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>44</v>
+      </c>
+      <c r="D153" t="s">
+        <v>11</v>
+      </c>
+      <c r="G153">
+        <v>2023</v>
+      </c>
+      <c r="H153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>121</v>
+      </c>
+      <c r="B154" t="s">
+        <v>128</v>
+      </c>
+      <c r="D154" t="s">
+        <v>16</v>
+      </c>
+      <c r="E154" t="s">
+        <v>28</v>
+      </c>
+      <c r="G154">
+        <v>2023</v>
+      </c>
+      <c r="H154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>41</v>
+      </c>
+      <c r="D155" t="s">
+        <v>42</v>
+      </c>
+      <c r="G155">
+        <v>2023</v>
+      </c>
+      <c r="H155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>14</v>
+      </c>
+      <c r="B156" t="s">
+        <v>37</v>
+      </c>
+      <c r="C156" t="s">
+        <v>129</v>
+      </c>
+      <c r="D156" t="s">
+        <v>16</v>
+      </c>
+      <c r="E156" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" t="s">
+        <v>111</v>
+      </c>
+      <c r="G156">
+        <v>2023</v>
+      </c>
+      <c r="H156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>90</v>
+      </c>
+      <c r="D157" t="s">
+        <v>61</v>
+      </c>
+      <c r="G157">
+        <v>2023</v>
+      </c>
+      <c r="H157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>130</v>
+      </c>
+      <c r="D158" t="s">
+        <v>178</v>
+      </c>
+      <c r="G158">
+        <v>2023</v>
+      </c>
+      <c r="H158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>130</v>
+      </c>
+      <c r="D159" t="s">
+        <v>178</v>
+      </c>
+      <c r="G159">
+        <v>2023</v>
+      </c>
+      <c r="H159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>126</v>
+      </c>
+      <c r="D160" t="s">
+        <v>127</v>
+      </c>
+      <c r="G160">
+        <v>2023</v>
+      </c>
+      <c r="H160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>82</v>
+      </c>
+      <c r="D161" t="s">
+        <v>61</v>
+      </c>
+      <c r="G161">
+        <v>2023</v>
+      </c>
+      <c r="H161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>132</v>
+      </c>
+      <c r="D162" t="s">
+        <v>9</v>
+      </c>
+      <c r="G162">
+        <v>2023</v>
+      </c>
+      <c r="H162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>133</v>
+      </c>
+      <c r="D163" t="s">
+        <v>134</v>
+      </c>
+      <c r="G163">
+        <v>2023</v>
+      </c>
+      <c r="H163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>135</v>
+      </c>
+      <c r="D164" t="s">
+        <v>9</v>
+      </c>
+      <c r="G164">
+        <v>2023</v>
+      </c>
+      <c r="H164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>136</v>
+      </c>
+      <c r="D165" t="s">
+        <v>137</v>
+      </c>
+      <c r="G165">
+        <v>2023</v>
+      </c>
+      <c r="H165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>135</v>
+      </c>
+      <c r="D166" t="s">
+        <v>9</v>
+      </c>
+      <c r="G166">
+        <v>2023</v>
+      </c>
+      <c r="H166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>138</v>
+      </c>
+      <c r="D167" t="s">
+        <v>139</v>
+      </c>
+      <c r="G167">
+        <v>2023</v>
+      </c>
+      <c r="H167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>57</v>
+      </c>
+      <c r="D168" t="s">
+        <v>58</v>
+      </c>
+      <c r="G168">
+        <v>2023</v>
+      </c>
+      <c r="H168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>18</v>
+      </c>
+      <c r="D169" t="s">
+        <v>19</v>
+      </c>
+      <c r="G169">
+        <v>2023</v>
+      </c>
+      <c r="H169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>125</v>
+      </c>
+      <c r="D170" t="s">
+        <v>111</v>
+      </c>
+      <c r="G170">
+        <v>2023</v>
+      </c>
+      <c r="H170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>140</v>
+      </c>
+      <c r="D171" t="s">
+        <v>9</v>
+      </c>
+      <c r="G171">
+        <v>2023</v>
+      </c>
+      <c r="H171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>135</v>
+      </c>
+      <c r="D172" t="s">
+        <v>9</v>
+      </c>
+      <c r="G172">
+        <v>2023</v>
+      </c>
+      <c r="H172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>141</v>
+      </c>
+      <c r="D173" t="s">
+        <v>9</v>
+      </c>
+      <c r="G173">
+        <v>2023</v>
+      </c>
+      <c r="H173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>142</v>
+      </c>
+      <c r="D174" t="s">
+        <v>9</v>
+      </c>
+      <c r="G174">
+        <v>2023</v>
+      </c>
+      <c r="H174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>143</v>
+      </c>
+      <c r="D175" t="s">
+        <v>11</v>
+      </c>
+      <c r="G175">
+        <v>2023</v>
+      </c>
+      <c r="H175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>144</v>
+      </c>
+      <c r="D176" t="s">
+        <v>7</v>
+      </c>
+      <c r="G176">
+        <v>2023</v>
+      </c>
+      <c r="H176">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>135</v>
+      </c>
+      <c r="D177" t="s">
+        <v>9</v>
+      </c>
+      <c r="G177">
+        <v>2023</v>
+      </c>
+      <c r="H177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>59</v>
+      </c>
+      <c r="D178" t="s">
+        <v>111</v>
+      </c>
+      <c r="G178">
+        <v>2023</v>
+      </c>
+      <c r="H178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>145</v>
+      </c>
+      <c r="D179" t="s">
+        <v>134</v>
+      </c>
+      <c r="G179">
+        <v>2023</v>
+      </c>
+      <c r="H179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>120</v>
+      </c>
+      <c r="D180" t="s">
+        <v>177</v>
+      </c>
+      <c r="G180">
+        <v>2023</v>
+      </c>
+      <c r="H180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>135</v>
+      </c>
+      <c r="D181" t="s">
+        <v>9</v>
+      </c>
+      <c r="G181">
+        <v>2023</v>
+      </c>
+      <c r="H181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>146</v>
+      </c>
+      <c r="D182" t="s">
+        <v>131</v>
+      </c>
+      <c r="G182">
+        <v>2023</v>
+      </c>
+      <c r="H182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>117</v>
+      </c>
+      <c r="D183" t="s">
+        <v>9</v>
+      </c>
+      <c r="G183">
+        <v>2023</v>
+      </c>
+      <c r="H183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>118</v>
+      </c>
+      <c r="D184" t="s">
+        <v>9</v>
+      </c>
+      <c r="G184">
+        <v>2023</v>
+      </c>
+      <c r="H184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>84</v>
+      </c>
+      <c r="D185" t="s">
+        <v>85</v>
+      </c>
+      <c r="G185">
+        <v>2023</v>
+      </c>
+      <c r="H185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>147</v>
+      </c>
+      <c r="D186" t="s">
+        <v>42</v>
+      </c>
+      <c r="G186">
+        <v>2023</v>
+      </c>
+      <c r="H186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>8</v>
+      </c>
+      <c r="D187" t="s">
+        <v>9</v>
+      </c>
+      <c r="G187">
+        <v>2023</v>
+      </c>
+      <c r="H187">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D188" t="s">
+        <v>61</v>
+      </c>
+      <c r="G188">
+        <v>2023</v>
+      </c>
+      <c r="H188">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>89</v>
+      </c>
+      <c r="D189" t="s">
+        <v>112</v>
+      </c>
+      <c r="G189">
+        <v>2023</v>
+      </c>
+      <c r="H189">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>8</v>
+      </c>
+      <c r="D190" t="s">
+        <v>9</v>
+      </c>
+      <c r="G190">
+        <v>2023</v>
+      </c>
+      <c r="H190">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>47</v>
+      </c>
+      <c r="D191" t="s">
+        <v>11</v>
+      </c>
+      <c r="G191">
+        <v>2023</v>
+      </c>
+      <c r="H191">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>82</v>
+      </c>
+      <c r="B192" t="s">
+        <v>14</v>
+      </c>
+      <c r="D192" t="s">
+        <v>61</v>
+      </c>
+      <c r="E192" t="s">
+        <v>16</v>
+      </c>
+      <c r="G192">
+        <v>2023</v>
+      </c>
+      <c r="H192">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>69</v>
+      </c>
+      <c r="D193" t="s">
+        <v>112</v>
+      </c>
+      <c r="G193">
+        <v>2023</v>
+      </c>
+      <c r="H193">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>69</v>
+      </c>
+      <c r="D194" t="s">
+        <v>112</v>
+      </c>
+      <c r="G194">
+        <v>2023</v>
+      </c>
+      <c r="H194">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>84</v>
+      </c>
+      <c r="D195" t="s">
+        <v>85</v>
+      </c>
+      <c r="G195">
+        <v>2023</v>
+      </c>
+      <c r="H195">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>121</v>
+      </c>
+      <c r="D196" t="s">
+        <v>16</v>
+      </c>
+      <c r="G196">
+        <v>2023</v>
+      </c>
+      <c r="H196">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>71</v>
+      </c>
+      <c r="D197" t="s">
+        <v>112</v>
+      </c>
+      <c r="G197">
+        <v>2023</v>
+      </c>
+      <c r="H197">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>123</v>
+      </c>
+      <c r="D198" t="s">
+        <v>124</v>
+      </c>
+      <c r="G198">
+        <v>2023</v>
+      </c>
+      <c r="H198">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>148</v>
+      </c>
+      <c r="D199" t="s">
+        <v>124</v>
+      </c>
+      <c r="G199">
+        <v>2023</v>
+      </c>
+      <c r="H199">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" t="s">
+        <v>7</v>
+      </c>
+      <c r="G200">
+        <v>2023</v>
+      </c>
+      <c r="H200">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>149</v>
+      </c>
+      <c r="D201" t="s">
+        <v>124</v>
+      </c>
+      <c r="G201">
+        <v>2023</v>
+      </c>
+      <c r="H201">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>148</v>
+      </c>
+      <c r="D202" t="s">
+        <v>124</v>
+      </c>
+      <c r="G202">
+        <v>2023</v>
+      </c>
+      <c r="H202">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>149</v>
+      </c>
+      <c r="D203" t="s">
+        <v>124</v>
+      </c>
+      <c r="G203">
+        <v>2023</v>
+      </c>
+      <c r="H203">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>71</v>
+      </c>
+      <c r="D204" t="s">
+        <v>112</v>
+      </c>
+      <c r="G204">
+        <v>2023</v>
+      </c>
+      <c r="H204">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>145</v>
+      </c>
+      <c r="D205" t="s">
+        <v>134</v>
+      </c>
+      <c r="G205">
+        <v>2023</v>
+      </c>
+      <c r="H205">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>149</v>
+      </c>
+      <c r="D206" t="s">
+        <v>124</v>
+      </c>
+      <c r="G206">
+        <v>2023</v>
+      </c>
+      <c r="H206">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>123</v>
+      </c>
+      <c r="D207" t="s">
+        <v>124</v>
+      </c>
+      <c r="G207">
+        <v>2023</v>
+      </c>
+      <c r="H207">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>148</v>
+      </c>
+      <c r="D208" t="s">
+        <v>124</v>
+      </c>
+      <c r="G208">
+        <v>2023</v>
+      </c>
+      <c r="H208">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>150</v>
+      </c>
+      <c r="B209" t="s">
+        <v>151</v>
+      </c>
+      <c r="D209" t="s">
+        <v>124</v>
+      </c>
+      <c r="E209" t="s">
+        <v>7</v>
+      </c>
+      <c r="G209">
+        <v>2023</v>
+      </c>
+      <c r="H209">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>96</v>
+      </c>
+      <c r="D210" t="s">
+        <v>36</v>
+      </c>
+      <c r="G210">
+        <v>2023</v>
+      </c>
+      <c r="H210">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>121</v>
+      </c>
+      <c r="D211" t="s">
+        <v>16</v>
+      </c>
+      <c r="G211">
+        <v>2023</v>
+      </c>
+      <c r="H211">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>38</v>
+      </c>
+      <c r="B212" t="s">
+        <v>14</v>
+      </c>
+      <c r="D212" t="s">
+        <v>39</v>
+      </c>
+      <c r="E212" t="s">
+        <v>16</v>
+      </c>
+      <c r="G212">
+        <v>2023</v>
+      </c>
+      <c r="H212">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>4</v>
+      </c>
+      <c r="D213" t="s">
+        <v>112</v>
+      </c>
+      <c r="G213">
+        <v>2023</v>
+      </c>
+      <c r="H213">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>47</v>
+      </c>
+      <c r="D214" t="s">
+        <v>11</v>
+      </c>
+      <c r="G214">
+        <v>2023</v>
+      </c>
+      <c r="H214">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>152</v>
+      </c>
+      <c r="D215" t="s">
+        <v>111</v>
+      </c>
+      <c r="G215">
+        <v>2023</v>
+      </c>
+      <c r="H215">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>8</v>
+      </c>
+      <c r="D216" t="s">
+        <v>9</v>
+      </c>
+      <c r="G216">
+        <v>2023</v>
+      </c>
+      <c r="H216">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>68</v>
+      </c>
+      <c r="D217" t="s">
+        <v>36</v>
+      </c>
+      <c r="G217">
+        <v>2023</v>
+      </c>
+      <c r="H217">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>153</v>
+      </c>
+      <c r="D218" t="s">
+        <v>134</v>
+      </c>
+      <c r="G218">
+        <v>2023</v>
+      </c>
+      <c r="H218">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>154</v>
+      </c>
+      <c r="D219" t="s">
+        <v>139</v>
+      </c>
+      <c r="G219">
+        <v>2023</v>
+      </c>
+      <c r="H219">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>155</v>
+      </c>
+      <c r="D220" t="s">
+        <v>112</v>
+      </c>
+      <c r="G220">
+        <v>2023</v>
+      </c>
+      <c r="H220">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>70</v>
+      </c>
+      <c r="B221" t="s">
+        <v>121</v>
+      </c>
+      <c r="D221" t="s">
+        <v>36</v>
+      </c>
+      <c r="E221" t="s">
+        <v>16</v>
+      </c>
+      <c r="G221">
+        <v>2023</v>
+      </c>
+      <c r="H221">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>156</v>
+      </c>
+      <c r="D222" t="s">
+        <v>131</v>
+      </c>
+      <c r="G222">
+        <v>2023</v>
+      </c>
+      <c r="H222">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>56</v>
+      </c>
+      <c r="D223" t="s">
+        <v>36</v>
+      </c>
+      <c r="G223">
+        <v>2023</v>
+      </c>
+      <c r="H223">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>157</v>
+      </c>
+      <c r="D224" t="s">
+        <v>113</v>
+      </c>
+      <c r="G224">
+        <v>2023</v>
+      </c>
+      <c r="H224">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>70</v>
+      </c>
+      <c r="B225" t="s">
+        <v>121</v>
+      </c>
+      <c r="D225" t="s">
+        <v>36</v>
+      </c>
+      <c r="E225" t="s">
+        <v>16</v>
+      </c>
+      <c r="G225">
+        <v>2023</v>
+      </c>
+      <c r="H225">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>121</v>
+      </c>
+      <c r="D226" t="s">
+        <v>16</v>
+      </c>
+      <c r="G226">
+        <v>2023</v>
+      </c>
+      <c r="H226">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>116</v>
+      </c>
+      <c r="D227" t="s">
+        <v>42</v>
+      </c>
+      <c r="G227">
+        <v>2023</v>
+      </c>
+      <c r="H227">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>142</v>
+      </c>
+      <c r="D228" t="s">
+        <v>9</v>
+      </c>
+      <c r="G228">
+        <v>2023</v>
+      </c>
+      <c r="H228">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>158</v>
+      </c>
+      <c r="D229" t="s">
+        <v>159</v>
+      </c>
+      <c r="G229">
+        <v>2023</v>
+      </c>
+      <c r="H229">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>152</v>
+      </c>
+      <c r="D230" t="s">
+        <v>111</v>
+      </c>
+      <c r="G230">
+        <v>2023</v>
+      </c>
+      <c r="H230">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>40</v>
+      </c>
+      <c r="D231" t="s">
+        <v>16</v>
+      </c>
+      <c r="G231">
+        <v>2023</v>
+      </c>
+      <c r="H231">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>160</v>
+      </c>
+      <c r="D232" t="s">
+        <v>42</v>
+      </c>
+      <c r="G232">
+        <v>2023</v>
+      </c>
+      <c r="H232">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>79</v>
+      </c>
+      <c r="D233" t="s">
+        <v>115</v>
+      </c>
+      <c r="G233">
+        <v>2023</v>
+      </c>
+      <c r="H233">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>60</v>
+      </c>
+      <c r="D234" t="s">
+        <v>61</v>
+      </c>
+      <c r="G234">
+        <v>2023</v>
+      </c>
+      <c r="H234">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>79</v>
+      </c>
+      <c r="D235" t="s">
+        <v>115</v>
+      </c>
+      <c r="G235">
+        <v>2023</v>
+      </c>
+      <c r="H235">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>40</v>
+      </c>
+      <c r="B236" t="s">
+        <v>161</v>
+      </c>
+      <c r="C236" t="s">
+        <v>162</v>
+      </c>
+      <c r="D236" t="s">
+        <v>16</v>
+      </c>
+      <c r="E236" t="s">
+        <v>163</v>
+      </c>
+      <c r="F236" t="s">
+        <v>163</v>
+      </c>
+      <c r="G236">
+        <v>2023</v>
+      </c>
+      <c r="H236">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>160</v>
+      </c>
+      <c r="D237" t="s">
+        <v>42</v>
+      </c>
+      <c r="G237">
+        <v>2023</v>
+      </c>
+      <c r="H237">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>40</v>
+      </c>
+      <c r="B238" t="s">
+        <v>164</v>
+      </c>
+      <c r="D238" t="s">
+        <v>16</v>
+      </c>
+      <c r="E238" t="s">
+        <v>88</v>
+      </c>
+      <c r="G238">
+        <v>2023</v>
+      </c>
+      <c r="H238">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>165</v>
+      </c>
+      <c r="D239" t="s">
+        <v>137</v>
+      </c>
+      <c r="G239">
+        <v>2023</v>
+      </c>
+      <c r="H239">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>40</v>
+      </c>
+      <c r="B240" t="s">
+        <v>164</v>
+      </c>
+      <c r="D240" t="s">
+        <v>16</v>
+      </c>
+      <c r="E240" t="s">
+        <v>88</v>
+      </c>
+      <c r="G240">
+        <v>2023</v>
+      </c>
+      <c r="H240">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>166</v>
+      </c>
+      <c r="D241" t="s">
+        <v>167</v>
+      </c>
+      <c r="G241">
+        <v>2023</v>
+      </c>
+      <c r="H241">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>5</v>
+      </c>
+      <c r="D242" t="s">
+        <v>111</v>
+      </c>
+      <c r="G242">
+        <v>2023</v>
+      </c>
+      <c r="H242">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>130</v>
+      </c>
+      <c r="D243" t="s">
+        <v>178</v>
+      </c>
+      <c r="G243">
+        <v>2023</v>
+      </c>
+      <c r="H243">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>152</v>
+      </c>
+      <c r="D244" t="s">
+        <v>111</v>
+      </c>
+      <c r="G244">
+        <v>2023</v>
+      </c>
+      <c r="H244">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>147</v>
+      </c>
+      <c r="D245" t="s">
+        <v>42</v>
+      </c>
+      <c r="G245">
+        <v>2023</v>
+      </c>
+      <c r="H245">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>4</v>
+      </c>
+      <c r="D246" t="s">
+        <v>112</v>
+      </c>
+      <c r="G246">
+        <v>2023</v>
+      </c>
+      <c r="H246">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>152</v>
+      </c>
+      <c r="D247" t="s">
+        <v>111</v>
+      </c>
+      <c r="G247">
+        <v>2023</v>
+      </c>
+      <c r="H247">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>168</v>
+      </c>
+      <c r="D248" t="s">
+        <v>9</v>
+      </c>
+      <c r="G248">
+        <v>2023</v>
+      </c>
+      <c r="H248">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>70</v>
+      </c>
+      <c r="D249" t="s">
+        <v>36</v>
+      </c>
+      <c r="G249">
+        <v>2023</v>
+      </c>
+      <c r="H249">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>169</v>
+      </c>
+      <c r="D250" t="s">
+        <v>111</v>
+      </c>
+      <c r="G250">
+        <v>2023</v>
+      </c>
+      <c r="H250">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>147</v>
+      </c>
+      <c r="D251" t="s">
+        <v>42</v>
+      </c>
+      <c r="G251">
+        <v>2023</v>
+      </c>
+      <c r="H251">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>170</v>
+      </c>
+      <c r="D252" t="s">
+        <v>111</v>
+      </c>
+      <c r="G252">
+        <v>2023</v>
+      </c>
+      <c r="H252">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>171</v>
+      </c>
+      <c r="D253" t="s">
+        <v>3</v>
+      </c>
+      <c r="G253">
+        <v>2023</v>
+      </c>
+      <c r="H253">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>47</v>
+      </c>
+      <c r="D254" t="s">
+        <v>11</v>
+      </c>
+      <c r="G254">
+        <v>2023</v>
+      </c>
+      <c r="H254">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>50</v>
+      </c>
+      <c r="D255" t="s">
+        <v>28</v>
+      </c>
+      <c r="G255">
+        <v>2023</v>
+      </c>
+      <c r="H255">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>172</v>
+      </c>
+      <c r="D256" t="s">
+        <v>134</v>
+      </c>
+      <c r="G256">
+        <v>2023</v>
+      </c>
+      <c r="H256">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>37</v>
+      </c>
+      <c r="D257" t="s">
+        <v>11</v>
+      </c>
+      <c r="G257">
+        <v>2023</v>
+      </c>
+      <c r="H257">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>173</v>
+      </c>
+      <c r="D258" t="s">
+        <v>163</v>
+      </c>
+      <c r="G258">
+        <v>2023</v>
+      </c>
+      <c r="H258">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>50</v>
+      </c>
+      <c r="D259" t="s">
+        <v>28</v>
+      </c>
+      <c r="G259">
+        <v>2023</v>
+      </c>
+      <c r="H259">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>47</v>
+      </c>
+      <c r="B260" t="s">
+        <v>174</v>
+      </c>
+      <c r="D260" t="s">
+        <v>11</v>
+      </c>
+      <c r="E260" t="s">
+        <v>11</v>
+      </c>
+      <c r="G260">
+        <v>2023</v>
+      </c>
+      <c r="H260">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>147</v>
+      </c>
+      <c r="D261" t="s">
+        <v>42</v>
+      </c>
+      <c r="G261">
+        <v>2023</v>
+      </c>
+      <c r="H261">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>142</v>
+      </c>
+      <c r="D262" t="s">
+        <v>9</v>
+      </c>
+      <c r="G262">
+        <v>2023</v>
+      </c>
+      <c r="H262">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>135</v>
+      </c>
+      <c r="D263" t="s">
+        <v>9</v>
+      </c>
+      <c r="G263">
+        <v>2023</v>
+      </c>
+      <c r="H263">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>172</v>
+      </c>
+      <c r="D264" t="s">
+        <v>134</v>
+      </c>
+      <c r="G264">
+        <v>2023</v>
+      </c>
+      <c r="H264">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>147</v>
+      </c>
+      <c r="D265" t="s">
+        <v>42</v>
+      </c>
+      <c r="G265">
+        <v>2023</v>
+      </c>
+      <c r="H265">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>175</v>
+      </c>
+      <c r="D266" t="s">
+        <v>81</v>
+      </c>
+      <c r="G266">
+        <v>2023</v>
+      </c>
+      <c r="H266">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>38</v>
+      </c>
+      <c r="B267" t="s">
+        <v>176</v>
+      </c>
+      <c r="D267" t="s">
+        <v>39</v>
+      </c>
+      <c r="E267" t="s">
+        <v>9</v>
+      </c>
+      <c r="G267">
+        <v>2023</v>
+      </c>
+      <c r="H267">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>